<commit_message>
Added video tutorials on topic: Git & Github (commands)
</commit_message>
<xml_diff>
--- a/Video tutorials/Git Github.xlsx
+++ b/Video tutorials/Git Github.xlsx
@@ -1,91 +1,116 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111ar\Desktop\Github repo\CodingEasy\Video tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911FA485-CA5B-4463-8EDA-CB7E49E4EC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{911FA485-CA5B-4463-8EDA-CB7E49E4EC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E70C3779-6A84-403C-BE1B-F7CB77CACEC0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Git Github</t>
+  </si>
+  <si>
+    <t>Utkarsh Rai</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>GD link</t>
+  </si>
+  <si>
+    <t>Youtube link</t>
+  </si>
+  <si>
+    <t>Introduction to Git &amp; Github</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1OzNETc6oe5tDewQivYgt0elq6NfQ0BRz/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git status command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RRFCBk8WkjKQj91gcCRLCrFmAXOpLVo0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git add command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1yBP7n8PpCNyAX4891f0uQ8FIk9brSEDg/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git init command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1NuG7XGedxh919clWwoaQYo33TTC0WhZ_/view</t>
+  </si>
+  <si>
+    <t>Pull Request 2 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git checkout command </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1_5D4bIORFzLN18LDjj7bO9uhF9TFJ8_6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git commit command</t>
+  </si>
   <si>
     <t>https://drive.google.com/file/d/1Q_wcBNGOJTEXDwXPye8OW8TXdkjtzEY0/view?usp=sharing</t>
   </si>
   <si>
-    <t>git commit command</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1_5D4bIORFzLN18LDjj7bO9uhF9TFJ8_6/view?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git checkout command </t>
-  </si>
-  <si>
-    <t>Pull Request 2 :</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1NuG7XGedxh919clWwoaQYo33TTC0WhZ_/view</t>
-  </si>
-  <si>
-    <t>git init command</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1yBP7n8PpCNyAX4891f0uQ8FIk9brSEDg/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>git add command</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1RRFCBk8WkjKQj91gcCRLCrFmAXOpLVo0/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>git status command</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1OzNETc6oe5tDewQivYgt0elq6NfQ0BRz/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Introduction to Git &amp; Github</t>
-  </si>
-  <si>
-    <t>Youtube link</t>
-  </si>
-  <si>
-    <t>GD link</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Utkarsh Rai</t>
-  </si>
-  <si>
-    <t>Git Github</t>
+    <t>Pull Request 3 :</t>
+  </si>
+  <si>
+    <t>git branch command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EicC-7Y0EWyOC_GZoFwkSCuFiFskn6Hi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git log command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1kjxST2z_KyeUqAHRPN4_hn6SFRp-Ye8C/view?usp=sharing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +183,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,100 +472,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="82.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -549,6 +594,8 @@
     <hyperlink ref="C8" r:id="rId4" xr:uid="{93475195-6B88-464F-AB04-F979C1936A61}"/>
     <hyperlink ref="C12" r:id="rId5" xr:uid="{5DF962F0-5DD4-4603-A09C-A772AD519B4A}"/>
     <hyperlink ref="C11" r:id="rId6" xr:uid="{819AA698-DC2D-4BC7-8046-4C97D9142020}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{829BF5A3-98A7-403C-B831-081C84284F56}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{05B29A96-F949-4B7B-9EB3-A5E72266DBD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added yt links in excel of git
</commit_message>
<xml_diff>
--- a/Video tutorials/Git Github.xlsx
+++ b/Video tutorials/Git Github.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111ar\Desktop\Github repo\CodingEasy\Video tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{911FA485-CA5B-4463-8EDA-CB7E49E4EC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E70C3779-6A84-403C-BE1B-F7CB77CACEC0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE28A70-0490-466B-BC7A-24DD5F153843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Git Github</t>
   </si>
@@ -104,13 +102,25 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1kjxST2z_KyeUqAHRPN4_hn6SFRp-Ye8C/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://youtu.be/WD5Un8e3EXQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gg1fX1t5OkA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/or4SKW0pwBY</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1fSfcE1hhzI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,26 +485,26 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -508,44 +518,56 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -553,7 +575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -561,16 +583,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -578,7 +600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added video tutorials on topic
</commit_message>
<xml_diff>
--- a/Video tutorials/Git Github.xlsx
+++ b/Video tutorials/Git Github.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111ar\Desktop\Github repo\CodingEasy\Video tutorials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cebd97a4bf8e4fa1/Desktop/New folder/CodingEasy/Video tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE28A70-0490-466B-BC7A-24DD5F153843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{3CE28A70-0490-466B-BC7A-24DD5F153843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15B7B93D-2BFE-4FD0-BF24-8886C29901F8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Git Github</t>
   </si>
@@ -114,6 +114,21 @@
   </si>
   <si>
     <t>https://youtu.be/1fSfcE1hhzI</t>
+  </si>
+  <si>
+    <t>Pull Request 4:</t>
+  </si>
+  <si>
+    <t>gitignore command</t>
+  </si>
+  <si>
+    <t>git diff command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1hSmhbMRXrPMPOj8Q5qEysc0L53-3dP1J/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1MwV1Isweru4x1E1YFr6yL91HEI-Z_AL9/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -482,29 +497,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="82.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -518,7 +533,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -529,7 +544,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -540,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -551,7 +566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -562,12 +577,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -575,7 +590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -583,16 +598,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -600,12 +615,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>